<commit_message>
CN0607: Escaleta, ajuste de tipo de motor
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion07/Escaleta_CN_06_07_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion07/Escaleta_CN_06_07_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado06\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="9213"/>
   </bookViews>
   <sheets>
     <sheet name="CN_06_07_CO" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CN_06_07_CO!$A$2:$U$38</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="250">
   <si>
     <t>Asignatura</t>
   </si>
@@ -775,6 +775,9 @@
   </si>
   <si>
     <t>RM_01_02_CO</t>
+  </si>
+  <si>
+    <t>m101A</t>
   </si>
 </sst>
 </file>
@@ -1091,25 +1094,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1131,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1464,128 +1467,128 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="U27" sqref="U27"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7" style="10" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="10" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="32.59765625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="4.1328125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="4.1328125" style="12" customWidth="1"/>
     <col min="10" max="10" width="61" style="10" customWidth="1"/>
     <col min="11" max="11" width="17" style="10" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.59765625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="13.86328125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="15.59765625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="29.265625" style="4" customWidth="1"/>
     <col min="16" max="16" width="7" style="27" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.1328125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.1328125" customWidth="1"/>
+    <col min="19" max="19" width="9.59765625" customWidth="1"/>
+    <col min="20" max="20" width="15.3984375" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="43"/>
+      <c r="O1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="48" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="43"/>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="38"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="7" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="36"/>
-    </row>
-    <row r="3" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="48"/>
+    </row>
+    <row r="3" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
         <v>122</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="13" t="s">
         <v>122</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A5" s="13" t="s">
         <v>122</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="13" t="s">
         <v>122</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A7" s="13" t="s">
         <v>122</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -1905,7 +1908,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="28"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A9" s="13" t="s">
         <v>122</v>
       </c>
@@ -1938,7 +1941,7 @@
       <c r="T9" s="30"/>
       <c r="U9" s="28"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>122</v>
       </c>
@@ -2032,7 +2035,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="28"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A12" s="13" t="s">
         <v>122</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="13" t="s">
         <v>122</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="13" t="s">
         <v>122</v>
       </c>
@@ -2211,7 +2214,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A15" s="13" t="s">
         <v>122</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="13" t="s">
         <v>122</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A17" s="13" t="s">
         <v>122</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="13" t="s">
         <v>122</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A19" s="13" t="s">
         <v>122</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A20" s="13" t="s">
         <v>122</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A21" s="13" t="s">
         <v>122</v>
       </c>
@@ -2590,7 +2593,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="28"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A22" s="13" t="s">
         <v>122</v>
       </c>
@@ -2623,7 +2626,7 @@
       <c r="T22" s="30"/>
       <c r="U22" s="28"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A23" s="13" t="s">
         <v>122</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A24" s="13" t="s">
         <v>122</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A25" s="13" t="s">
         <v>122</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A26" s="13" t="s">
         <v>122</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A27" s="13" t="s">
         <v>122</v>
       </c>
@@ -2916,7 +2919,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A28" s="13" t="s">
         <v>122</v>
       </c>
@@ -2949,7 +2952,7 @@
       <c r="T28" s="30"/>
       <c r="U28" s="28"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A29" s="13" t="s">
         <v>122</v>
       </c>
@@ -2982,7 +2985,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="28"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A30" s="13" t="s">
         <v>122</v>
       </c>
@@ -3015,7 +3018,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="28"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A31" s="13" t="s">
         <v>122</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A32" s="13" t="s">
         <v>122</v>
       </c>
@@ -3111,7 +3114,7 @@
       </c>
       <c r="M32" s="24"/>
       <c r="N32" s="24" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="O32" s="24"/>
       <c r="P32" s="24" t="s">
@@ -3133,7 +3136,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A33" s="13" t="s">
         <v>122</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A34" s="13" t="s">
         <v>122</v>
       </c>
@@ -3247,7 +3250,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A35" s="13" t="s">
         <v>122</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A36" s="13" t="s">
         <v>122</v>
       </c>
@@ -3345,7 +3348,7 @@
       <c r="T36" s="30"/>
       <c r="U36" s="28"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A37" s="13" t="s">
         <v>122</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" s="10" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A38" s="13" t="s">
         <v>122</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>94</v>
       </c>
@@ -3477,7 +3480,7 @@
       <c r="P81" s="26"/>
       <c r="Q81"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>95</v>
       </c>
@@ -3493,7 +3496,7 @@
       <c r="P82" s="26"/>
       <c r="Q82"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>96</v>
       </c>
@@ -3509,7 +3512,7 @@
       <c r="P83" s="26"/>
       <c r="Q83"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A84" s="10" t="s">
         <v>97</v>
       </c>
@@ -3525,7 +3528,7 @@
       <c r="P84" s="26"/>
       <c r="Q84"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A85" s="10" t="s">
         <v>98</v>
       </c>
@@ -3541,7 +3544,7 @@
       <c r="P85" s="26"/>
       <c r="Q85"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A86" s="10" t="s">
         <v>99</v>
       </c>
@@ -3557,7 +3560,7 @@
       <c r="P86" s="26"/>
       <c r="Q86"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A87" s="10" t="s">
         <v>101</v>
       </c>
@@ -3573,7 +3576,7 @@
       <c r="P87" s="26"/>
       <c r="Q87"/>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A88" s="10" t="s">
         <v>100</v>
       </c>
@@ -3589,7 +3592,7 @@
       <c r="P88" s="26"/>
       <c r="Q88"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A89" s="10" t="s">
         <v>102</v>
       </c>
@@ -3605,7 +3608,7 @@
       <c r="P89" s="26"/>
       <c r="Q89"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A90" s="10" t="s">
         <v>103</v>
       </c>
@@ -3621,7 +3624,7 @@
       <c r="P90" s="26"/>
       <c r="Q90"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A91" s="10" t="s">
         <v>104</v>
       </c>
@@ -3637,7 +3640,7 @@
       <c r="P91" s="26"/>
       <c r="Q91"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A92" s="10" t="s">
         <v>105</v>
       </c>
@@ -3653,7 +3656,7 @@
       <c r="P92" s="26"/>
       <c r="Q92"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A93" s="10" t="s">
         <v>106</v>
       </c>
@@ -3669,7 +3672,7 @@
       <c r="P93" s="26"/>
       <c r="Q93"/>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A94" s="10" t="s">
         <v>107</v>
       </c>
@@ -3685,7 +3688,7 @@
       <c r="P94" s="26"/>
       <c r="Q94"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A95" s="10" t="s">
         <v>108</v>
       </c>
@@ -3701,7 +3704,7 @@
       <c r="P95" s="26"/>
       <c r="Q95"/>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A96" s="10" t="s">
         <v>67</v>
       </c>
@@ -3717,7 +3720,7 @@
       <c r="P96" s="26"/>
       <c r="Q96"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A97" s="10" t="s">
         <v>68</v>
       </c>
@@ -3733,7 +3736,7 @@
       <c r="P97" s="26"/>
       <c r="Q97"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A98" s="10" t="s">
         <v>69</v>
       </c>
@@ -3750,7 +3753,7 @@
       <c r="P98" s="26"/>
       <c r="Q98"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A99" s="10" t="s">
         <v>70</v>
       </c>
@@ -3767,7 +3770,7 @@
       <c r="P99" s="26"/>
       <c r="Q99"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A100" s="10" t="s">
         <v>71</v>
       </c>
@@ -3784,7 +3787,7 @@
       <c r="P100" s="26"/>
       <c r="Q100"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A101" s="10" t="s">
         <v>72</v>
       </c>
@@ -3801,7 +3804,7 @@
       <c r="P101" s="26"/>
       <c r="Q101"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A102" s="10" t="s">
         <v>73</v>
       </c>
@@ -3818,7 +3821,7 @@
       <c r="P102" s="26"/>
       <c r="Q102"/>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A103" s="10" t="s">
         <v>74</v>
       </c>
@@ -3835,7 +3838,7 @@
       <c r="P103" s="26"/>
       <c r="Q103"/>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A104" s="10" t="s">
         <v>75</v>
       </c>
@@ -3852,7 +3855,7 @@
       <c r="P104" s="26"/>
       <c r="Q104"/>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A105" s="10" t="s">
         <v>76</v>
       </c>
@@ -3869,7 +3872,7 @@
       <c r="P105" s="26"/>
       <c r="Q105"/>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A106" s="10" t="s">
         <v>77</v>
       </c>
@@ -3886,7 +3889,7 @@
       <c r="P106" s="26"/>
       <c r="Q106"/>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A107" s="10" t="s">
         <v>78</v>
       </c>
@@ -3903,7 +3906,7 @@
       <c r="P107" s="26"/>
       <c r="Q107"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A108" s="10" t="s">
         <v>79</v>
       </c>
@@ -3920,7 +3923,7 @@
       <c r="P108" s="26"/>
       <c r="Q108"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A109" s="10" t="s">
         <v>80</v>
       </c>
@@ -3937,7 +3940,7 @@
       <c r="P109" s="26"/>
       <c r="Q109"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A110" s="10" t="s">
         <v>81</v>
       </c>
@@ -3954,7 +3957,7 @@
       <c r="P110" s="26"/>
       <c r="Q110"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A111" s="10" t="s">
         <v>82</v>
       </c>
@@ -3971,7 +3974,7 @@
       <c r="P111" s="26"/>
       <c r="Q111"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A112" s="10" t="s">
         <v>83</v>
       </c>
@@ -3988,7 +3991,7 @@
       <c r="P112" s="26"/>
       <c r="Q112"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A113" s="10" t="s">
         <v>84</v>
       </c>
@@ -4005,7 +4008,7 @@
       <c r="P113" s="26"/>
       <c r="Q113"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A114" s="10" t="s">
         <v>85</v>
       </c>
@@ -4022,7 +4025,7 @@
       <c r="P114" s="26"/>
       <c r="Q114"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A115" s="10" t="s">
         <v>86</v>
       </c>
@@ -4039,7 +4042,7 @@
       <c r="P115" s="26"/>
       <c r="Q115"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A116" s="10" t="s">
         <v>118</v>
       </c>
@@ -4056,7 +4059,7 @@
       <c r="P116" s="26"/>
       <c r="Q116"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A117" s="10" t="s">
         <v>117</v>
       </c>
@@ -4076,6 +4079,12 @@
   </sheetData>
   <autoFilter ref="A2:U38"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4090,12 +4099,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I37 P3:P38">
@@ -4114,7 +4117,7 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N37 M37</xm:sqref>
+          <xm:sqref>M37 N3:N31 N33:N37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4161,27 +4164,27 @@
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="5" customWidth="1"/>
     <col min="4" max="4" width="34" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.86328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" style="5" customWidth="1"/>
     <col min="7" max="7" width="18" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.73046875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="5" customWidth="1"/>
     <col min="12" max="12" width="17" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="5"/>
-    <col min="14" max="14" width="24.28515625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="5"/>
+    <col min="13" max="13" width="11.3984375" style="5"/>
+    <col min="14" max="14" width="24.265625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="69.86328125" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.3984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -4198,7 +4201,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -4222,7 +4225,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -4241,7 +4244,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -4260,7 +4263,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -4276,7 +4279,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -4293,7 +4296,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -4310,7 +4313,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -4325,7 +4328,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -4340,7 +4343,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -4355,7 +4358,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -4370,7 +4373,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -4385,7 +4388,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -4400,7 +4403,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -4415,7 +4418,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -4430,7 +4433,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -4445,7 +4448,7 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5" t="s">
@@ -4459,7 +4462,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5" t="s">
@@ -4473,7 +4476,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5" t="s">
@@ -4487,7 +4490,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5" t="s">
@@ -4501,7 +4504,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -4516,7 +4519,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -4531,7 +4534,7 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -4546,7 +4549,7 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -4561,7 +4564,7 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -4576,7 +4579,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -4591,7 +4594,7 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -4606,7 +4609,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -4621,7 +4624,7 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -4636,7 +4639,7 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -4651,7 +4654,7 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -4666,7 +4669,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -4681,7 +4684,7 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -4696,7 +4699,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -4711,7 +4714,7 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -4726,7 +4729,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -4741,7 +4744,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -4756,7 +4759,7 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -4771,7 +4774,7 @@
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -4786,7 +4789,7 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -4801,7 +4804,7 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -4816,7 +4819,7 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -4831,7 +4834,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -4846,7 +4849,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -4861,7 +4864,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -4876,7 +4879,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -4891,7 +4894,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -4906,7 +4909,7 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -4921,7 +4924,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -4933,7 +4936,7 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -4945,7 +4948,7 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -4958,7 +4961,7 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -4971,7 +4974,7 @@
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -4984,7 +4987,7 @@
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -4997,7 +5000,7 @@
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -5010,7 +5013,7 @@
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -5023,7 +5026,7 @@
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -5036,7 +5039,7 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -5049,7 +5052,7 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -5062,7 +5065,7 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -5075,7 +5078,7 @@
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -5088,7 +5091,7 @@
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
@@ -5101,7 +5104,7 @@
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -5114,7 +5117,7 @@
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
@@ -5127,7 +5130,7 @@
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
@@ -5140,7 +5143,7 @@
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
@@ -5153,7 +5156,7 @@
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
@@ -5166,7 +5169,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -5179,7 +5182,7 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -5192,7 +5195,7 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -5205,7 +5208,7 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5219,7 +5222,7 @@
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -5233,7 +5236,7 @@
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -5247,7 +5250,7 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -5261,7 +5264,7 @@
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -5275,7 +5278,7 @@
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -5289,7 +5292,7 @@
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -5303,7 +5306,7 @@
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -5317,7 +5320,7 @@
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -5331,7 +5334,7 @@
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -5345,7 +5348,7 @@
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -5359,7 +5362,7 @@
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -5373,7 +5376,7 @@
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -5387,7 +5390,7 @@
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -5401,7 +5404,7 @@
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -5415,7 +5418,7 @@
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -5429,7 +5432,7 @@
       <c r="K86" s="6"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -5443,7 +5446,7 @@
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -5457,7 +5460,7 @@
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -5471,7 +5474,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -5485,7 +5488,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -5499,7 +5502,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -5513,7 +5516,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -5527,7 +5530,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -5541,7 +5544,7 @@
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -5555,7 +5558,7 @@
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -5569,7 +5572,7 @@
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -5583,7 +5586,7 @@
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -5597,7 +5600,7 @@
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -5611,7 +5614,7 @@
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -5625,7 +5628,7 @@
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -5639,7 +5642,7 @@
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
@@ -5653,7 +5656,7 @@
       <c r="K102" s="6"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -5667,7 +5670,7 @@
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -5681,7 +5684,7 @@
       <c r="K104" s="6"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -5695,7 +5698,7 @@
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -5709,7 +5712,7 @@
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -5723,7 +5726,7 @@
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -5737,7 +5740,7 @@
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -5751,7 +5754,7 @@
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -5765,7 +5768,7 @@
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -5779,7 +5782,7 @@
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -5793,7 +5796,7 @@
       <c r="K112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -5807,7 +5810,7 @@
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -5821,7 +5824,7 @@
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -5835,7 +5838,7 @@
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -5849,7 +5852,7 @@
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -5863,7 +5866,7 @@
       <c r="K117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -5877,7 +5880,7 @@
       <c r="K118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -5891,7 +5894,7 @@
       <c r="K119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -5905,7 +5908,7 @@
       <c r="K120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -5919,7 +5922,7 @@
       <c r="K121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -5933,7 +5936,7 @@
       <c r="K122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -5947,7 +5950,7 @@
       <c r="K123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -5961,7 +5964,7 @@
       <c r="K124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
@@ -5975,7 +5978,7 @@
       <c r="K125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -5989,7 +5992,7 @@
       <c r="K126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
@@ -6003,7 +6006,7 @@
       <c r="K127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
@@ -6017,7 +6020,7 @@
       <c r="K128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -6031,7 +6034,7 @@
       <c r="K129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
@@ -6045,7 +6048,7 @@
       <c r="K130" s="6"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
@@ -6059,7 +6062,7 @@
       <c r="K131" s="6"/>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
@@ -6073,7 +6076,7 @@
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>

</xml_diff>